<commit_message>
updated region + new region_cont xlsx
</commit_message>
<xml_diff>
--- a/excels/lite/RegionDF.xlsx
+++ b/excels/lite/RegionDF.xlsx
@@ -423,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>92.57894736842105</v>
+        <v>93.1875</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -431,7 +431,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>73.73684210526316</v>
+        <v>76.84375</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -439,7 +439,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>15.05263157894737</v>
+        <v>15.09375</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -447,7 +447,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>13.10526315789474</v>
+        <v>13.71875</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -455,7 +455,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>12.78947368421053</v>
+        <v>12.6875</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -463,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>9.052631578947368</v>
+        <v>9.09375</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -471,7 +471,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>8.315789473684211</v>
+        <v>9.09375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW EXCELS 16/4 and bug fix @ regions
</commit_message>
<xml_diff>
--- a/excels/lite/RegionDF.xlsx
+++ b/excels/lite/RegionDF.xlsx
@@ -397,7 +397,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>96.36206896551724</v>
+        <v>96.37931034482759</v>
       </c>
     </row>
     <row r="3">
@@ -407,7 +407,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83.98275862068965</v>
+        <v>83.96551724137932</v>
       </c>
     </row>
     <row r="4">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10.05172413793103</v>
+        <v>10.08620689655172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed fetch regions to have the latest and not the mean values
</commit_message>
<xml_diff>
--- a/excels/lite/RegionDF.xlsx
+++ b/excels/lite/RegionDF.xlsx
@@ -1,41 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgosandreou/Documents/Visual Studio/thesis-old/excels/lite/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21800" windowHeight="10940"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Fans</t>
+  </si>
+  <si>
+    <t>Attica (region), Greece</t>
+  </si>
+  <si>
+    <t>Central Macedonia, Greece</t>
+  </si>
+  <si>
+    <t>Thessaly, Greece</t>
+  </si>
+  <si>
+    <t>Western Greece, Greece</t>
+  </si>
+  <si>
+    <t>Eastern Macedonia and Thrace, Greece</t>
+  </si>
+  <si>
+    <t>Central Greece (region), Greece</t>
+  </si>
+  <si>
+    <t>Crete, Greece</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,18 +107,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -365,102 +412,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Regions</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Fans</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Central Macedonia, Greece</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>96.55932203389831</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Attica (region), Greece</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>84.49152542372882</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Thessaly, Greece</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>17.61016949152542</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Western Greece, Greece</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>15.35593220338983</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Epirus (region), Greece</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>13.25423728813559</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Eastern Macedonia and Thrace, Greece</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>11.32203389830508</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Crete, Greece</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>10.15254237288136</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>